<commit_message>
Changed scintillator temp sensor
</commit_message>
<xml_diff>
--- a/hardware/Eagle Designs/Scintillator Detector/Main PCB BOM.xlsx
+++ b/hardware/Eagle Designs/Scintillator Detector/Main PCB BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahumo\Documents\5_UHFall2021\epet401\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8FCD37-C9FB-4656-A7FB-0C8A9A731EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5F507D-E228-4FD9-84F0-18BF0A0E86CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB625052-FCA8-4B3F-8524-05803AA61B5F}"/>
   </bookViews>
@@ -167,9 +167,6 @@
     <t>U3</t>
   </si>
   <si>
-    <t>TMP36GSZ</t>
-  </si>
-  <si>
     <t>C2, C9</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>45.3k</t>
+  </si>
+  <si>
+    <t>TMP36FSZ</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,7 +620,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -698,7 +698,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>16</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>17</v>
@@ -776,7 +776,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>28</v>
@@ -789,7 +789,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>29</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>30</v>
@@ -844,7 +844,7 @@
         <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>25</v>
@@ -883,10 +883,10 @@
         <v>40</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>

</xml_diff>